<commit_message>
Changed some statistics for part 1
</commit_message>
<xml_diff>
--- a/results/part1/stats.xlsx
+++ b/results/part1/stats.xlsx
@@ -7,7 +7,12 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="eil51" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="berlin52" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="pr136" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="pr226" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="d198" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="mean" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -462,6 +467,401 @@
         </is>
       </c>
       <c r="B2" t="n">
+        <v>0.8304121401559936</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.899677890294611</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.8188253837210422</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.601256411976037</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>min</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.02623362030768031</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.03391590397004692</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.01968897357784272</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.02395574176995417</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>random</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>bayesian</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>forest</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>gradient</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>auc</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0.3470775386038567</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.6504245201931586</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.2266698501351931</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.1590209092862858</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>min</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.0007518913878295021</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.01900986082063078</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.004513743086632056</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.003085628744123837</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>random</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>bayesian</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>forest</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>gradient</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>auc</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>2.265570492570207</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1.849572900070808</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1.809140861395097</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1.947604744127015</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>min</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.09676929003141378</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.09267605715685522</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.07540059859748173</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.07542778875383883</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>random</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>bayesian</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>forest</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>gradient</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>auc</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>1.837164294898639</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1.394382597025814</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1.54691092308816</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1.497230361062779</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>min</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.07454252915968133</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.07226467000338908</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.07155621950623137</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.04211928288038776</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>random</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>bayesian</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>forest</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>gradient</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>auc</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>2.138673722391764</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1.697629530878448</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1.940128028161632</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1.745387991281444</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>min</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.09220523859069986</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.08204043426292522</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.08460608390260768</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.08085682164963927</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>random</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>bayesian</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>forest</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>gradient</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>auc</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
         <v>1.483779637724092</v>
       </c>
       <c r="C2" t="n">

</xml_diff>